<commit_message>
Made rebuilds faster by only build cjxl and djxl during GA
</commit_message>
<xml_diff>
--- a/W-OP8/data/output/spreadsheets/Kodak_Lossless_True_Color_Image_Suite_tr0.1_max10_p10_g3_m0.05_x0.9_e2_t3_results.xlsx
+++ b/W-OP8/data/output/spreadsheets/Kodak_Lossless_True_Color_Image_Suite_tr0.1_max10_p10_g3_m0.05_x0.9_e2_t3_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xavierhillroy/Desktop/Super/Brains/Academic/Western/Year_5/Fall_term/thesis/libjxl-wop8/W-OP8/data/output/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA37D764-735E-A545-8180-672BAA0F91A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4923AF-0D15-4C48-ADB4-6CE8340A74BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" r:id="rId1"/>
@@ -1341,9 +1341,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2389,7 +2397,7 @@
         <v>177485</v>
       </c>
       <c r="M24">
-        <v>0.16413370768229171</v>
+        <v>0.16413370768229199</v>
       </c>
       <c r="N24">
         <v>1.9102392740262371</v>
@@ -2404,17 +2412,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -3564,7 +3581,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>